<commit_message>
Updating standings, haven't run clean scripts
</commit_message>
<xml_diff>
--- a/training_data/2004/2004_basic_hitting.xlsx
+++ b/training_data/2004/2004_basic_hitting.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex_1/Desktop/MVP-Predictor/training_data/2004/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EC9205-2754-4B44-AB5A-EF5BF4DF49EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE51BE3-0A74-FD48-ADDC-CFDF25D56614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{2E9DBF92-5F53-6F43-B8BF-E1975E6119BA}"/>
+    <workbookView xWindow="5920" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{2E9DBF92-5F53-6F43-B8BF-E1975E6119BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3930,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1683A667-CF6A-9045-B907-BC3ADF7EAC4B}">
   <dimension ref="A1:J1314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>